<commit_message>
next adjacent slot vacancy fillup
</commit_message>
<xml_diff>
--- a/Book11.xlsx
+++ b/Book11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="22188" windowHeight="8555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1236,10 +1236,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1333,8 +1333,6 @@
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1">
         <v>13</v>
@@ -1362,8 +1360,6 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="1">
         <v>15</v>
@@ -1391,10 +1387,7 @@
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
       <c r="J5" s="1">
         <v>40</v>
       </c>
@@ -1418,10 +1411,7 @@
       <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
       <c r="J6" s="1">
         <v>8</v>
       </c>
@@ -1445,9 +1435,6 @@
       <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
       <c r="I7" s="1">
         <v>16</v>
       </c>
@@ -1474,10 +1461,6 @@
       <c r="E8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
       <c r="J8" s="1">
         <v>10</v>
       </c>
@@ -1501,9 +1484,6 @@
       <c r="E9" s="2">
         <v>3</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
       <c r="I9" s="1">
         <v>16</v>
       </c>
@@ -1530,10 +1510,6 @@
       <c r="E10" s="2">
         <v>3</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
       <c r="J10" s="1">
         <v>35</v>
       </c>
@@ -1557,10 +1533,6 @@
       <c r="E11" s="2">
         <v>3</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
       <c r="J11" s="1">
         <v>15</v>
       </c>
@@ -1584,12 +1556,8 @@
       <c r="E12" s="2">
         <v>3</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
       <c r="J12" s="1">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K12" s="1">
         <v>13</v>
@@ -1611,9 +1579,6 @@
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
       <c r="I13" s="1">
         <v>17</v>
       </c>
@@ -1640,12 +1605,8 @@
       <c r="E14" s="2">
         <v>3</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
       <c r="J14" s="1">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="K14" s="1">
         <v>16</v>
@@ -1667,9 +1628,6 @@
       <c r="E15" s="2">
         <v>2</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
       <c r="I15" s="1">
         <v>15</v>
       </c>
@@ -1696,10 +1654,6 @@
       <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
       <c r="J16" s="1">
         <v>17</v>
       </c>
@@ -1723,10 +1677,6 @@
       <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
       <c r="J17" s="1">
         <v>60</v>
       </c>
@@ -1750,9 +1700,6 @@
       <c r="E18" s="2">
         <v>3</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
       <c r="I18" s="1">
         <v>16</v>
       </c>
@@ -1779,10 +1726,6 @@
       <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
       <c r="J19" s="1">
         <v>56</v>
       </c>
@@ -2065,7 +2008,7 @@
         <v>3</v>
       </c>
       <c r="J30" s="1">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K30" s="1">
         <v>13</v>
@@ -2114,7 +2057,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="1">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="K32" s="1">
         <v>16</v>
@@ -2516,7 +2459,7 @@
         <v>3</v>
       </c>
       <c r="J48" s="1">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="K48" s="1">
         <v>13</v>
@@ -2546,150 +2489,6 @@
       </c>
       <c r="K49" s="1">
         <v>15</v>
-      </c>
-    </row>
-    <row r="50" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A50" s="2">
-        <v>12102909</v>
-      </c>
-      <c r="B50" s="2">
-        <v>16</v>
-      </c>
-      <c r="C50" s="2">
-        <v>3</v>
-      </c>
-      <c r="D50" s="2">
-        <v>3</v>
-      </c>
-      <c r="E50" s="2">
-        <v>3</v>
-      </c>
-      <c r="J50" s="1">
-        <v>12</v>
-      </c>
-      <c r="K50" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A51" s="2">
-        <v>4343009</v>
-      </c>
-      <c r="B51" s="2">
-        <v>28</v>
-      </c>
-      <c r="C51" s="2">
-        <v>3</v>
-      </c>
-      <c r="D51" s="2">
-        <v>2</v>
-      </c>
-      <c r="E51" s="2">
-        <v>2</v>
-      </c>
-      <c r="I51" s="1">
-        <v>15</v>
-      </c>
-      <c r="J51" s="1">
-        <v>24</v>
-      </c>
-      <c r="K51" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A52" s="2">
-        <v>1171234</v>
-      </c>
-      <c r="B52" s="2">
-        <v>21</v>
-      </c>
-      <c r="C52" s="2">
-        <v>3</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2">
-        <v>3</v>
-      </c>
-      <c r="J52" s="1">
-        <v>17</v>
-      </c>
-      <c r="K52" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A53" s="2">
-        <v>76531113</v>
-      </c>
-      <c r="B53" s="2">
-        <v>65</v>
-      </c>
-      <c r="C53" s="2">
-        <v>3</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1</v>
-      </c>
-      <c r="E53" s="2">
-        <v>1</v>
-      </c>
-      <c r="J53" s="1">
-        <v>60</v>
-      </c>
-      <c r="K53" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A54" s="2">
-        <v>633312</v>
-      </c>
-      <c r="B54" s="2">
-        <v>84</v>
-      </c>
-      <c r="C54" s="2">
-        <v>3</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2">
-        <v>3</v>
-      </c>
-      <c r="I54" s="1">
-        <v>16</v>
-      </c>
-      <c r="J54" s="1">
-        <v>80</v>
-      </c>
-      <c r="K54" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:11">
-      <c r="A55" s="2">
-        <v>634862323</v>
-      </c>
-      <c r="B55" s="2">
-        <v>62</v>
-      </c>
-      <c r="C55" s="2">
-        <v>3</v>
-      </c>
-      <c r="D55" s="2">
-        <v>2</v>
-      </c>
-      <c r="E55" s="2">
-        <v>3</v>
-      </c>
-      <c r="J55" s="1">
-        <v>56</v>
-      </c>
-      <c r="K55" s="1">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>